<commit_message>
updates to models and new data from them
</commit_message>
<xml_diff>
--- a/experimental_models/combined_model_with_cpd43.xlsx
+++ b/experimental_models/combined_model_with_cpd43.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mihir/Library/CloudStorage/iCloud Drive/Documents/Summer/Models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{47101DEF-CCF5-AD4E-A51C-84C8AB18E471}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E27B174-8B14-D14A-B4A9-0152E3124D0A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28420" yWindow="-23540" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28420" yWindow="-23540" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="species" sheetId="1" r:id="rId1"/>
@@ -3096,8 +3096,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J124"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3172,7 +3172,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F3" s="7">
         <v>10</v>
@@ -6773,8 +6773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AZ175"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>